<commit_message>
new pdf report for skipped tc.
</commit_message>
<xml_diff>
--- a/test_scripts/chrome/QS004_demoqa_testscript.xlsx
+++ b/test_scripts/chrome/QS004_demoqa_testscript.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\allprojects\web_automation_htmltopdf\test_scripts\edge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\allprojects\web_automation_htmltopdf\test_scripts\chrome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729425B1-895A-4680-A6EA-86CCB3955AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562ADD36-73E5-4682-8DF9-8C174E2E9232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4369D99C-3FCA-451D-9ADF-0150CDA12363}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>open_browser</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>upload_file</t>
-  </si>
-  <si>
-    <t>chromedgerunonlinux.txt</t>
   </si>
 </sst>
 </file>
@@ -522,7 +519,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,9 +680,6 @@
       <c r="C14" t="s">
         <v>35</v>
       </c>
-      <c r="D14" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">

</xml_diff>